<commit_message>
Deployed 217f1df with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA 12S metab/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
+++ b/eDNA 12S metab/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
@@ -518,7 +518,7 @@
         <v>66</v>
       </c>
       <c r="G2">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="H2">
         <v>106</v>
@@ -622,7 +622,7 @@
         <v>66</v>
       </c>
       <c r="G3">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="H3">
         <v>106</v>
@@ -716,7 +716,7 @@
         <v>66</v>
       </c>
       <c r="G4">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="H4">
         <v>106</v>
@@ -2518,7 +2518,7 @@
         <v>122</v>
       </c>
       <c r="G24">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="H24">
         <v>105</v>
@@ -2572,7 +2572,7 @@
         <v>122</v>
       </c>
       <c r="G25">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="H25">
         <v>105</v>
@@ -2673,7 +2673,7 @@
         <v>122</v>
       </c>
       <c r="G26">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="H26">
         <v>105</v>
@@ -2727,7 +2727,7 @@
         <v>170</v>
       </c>
       <c r="G27">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H27">
         <v>107</v>
@@ -2831,7 +2831,7 @@
         <v>170</v>
       </c>
       <c r="G28">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H28">
         <v>107</v>
@@ -2935,7 +2935,7 @@
         <v>170</v>
       </c>
       <c r="G29">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H29">
         <v>107</v>
@@ -3435,7 +3435,7 @@
         <v>178</v>
       </c>
       <c r="G34">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H34">
         <v>107</v>
@@ -3539,7 +3539,7 @@
         <v>178</v>
       </c>
       <c r="G35">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H35">
         <v>107</v>
@@ -3643,7 +3643,7 @@
         <v>178</v>
       </c>
       <c r="G36">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H36">
         <v>107</v>
@@ -3747,7 +3747,7 @@
         <v>178</v>
       </c>
       <c r="G37">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H37">
         <v>107</v>
@@ -3851,7 +3851,7 @@
         <v>178</v>
       </c>
       <c r="G38">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H38">
         <v>107</v>
@@ -4160,7 +4160,7 @@
         <v>2273</v>
       </c>
       <c r="G41">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H41">
         <v>105</v>
@@ -4214,7 +4214,7 @@
         <v>2273</v>
       </c>
       <c r="G42">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H42">
         <v>105</v>
@@ -4315,7 +4315,7 @@
         <v>2273</v>
       </c>
       <c r="G43">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H43">
         <v>105</v>
@@ -4369,7 +4369,7 @@
         <v>579</v>
       </c>
       <c r="G44">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H44">
         <v>106</v>
@@ -4473,7 +4473,7 @@
         <v>579</v>
       </c>
       <c r="G45">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H45">
         <v>106</v>

</xml_diff>

<commit_message>
Deployed 3948e65 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA 12S metab/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
+++ b/eDNA 12S metab/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
@@ -518,7 +518,7 @@
         <v>66</v>
       </c>
       <c r="G2">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="H2">
         <v>106</v>
@@ -622,7 +622,7 @@
         <v>66</v>
       </c>
       <c r="G3">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="H3">
         <v>106</v>
@@ -716,7 +716,7 @@
         <v>66</v>
       </c>
       <c r="G4">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="H4">
         <v>106</v>
@@ -2727,7 +2727,7 @@
         <v>170</v>
       </c>
       <c r="G27">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H27">
         <v>107</v>
@@ -2831,7 +2831,7 @@
         <v>170</v>
       </c>
       <c r="G28">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H28">
         <v>107</v>
@@ -2935,7 +2935,7 @@
         <v>170</v>
       </c>
       <c r="G29">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H29">
         <v>107</v>
@@ -3435,7 +3435,7 @@
         <v>178</v>
       </c>
       <c r="G34">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H34">
         <v>107</v>
@@ -3539,7 +3539,7 @@
         <v>178</v>
       </c>
       <c r="G35">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H35">
         <v>107</v>
@@ -3643,7 +3643,7 @@
         <v>178</v>
       </c>
       <c r="G36">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H36">
         <v>107</v>
@@ -3747,7 +3747,7 @@
         <v>178</v>
       </c>
       <c r="G37">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H37">
         <v>107</v>
@@ -3851,7 +3851,7 @@
         <v>178</v>
       </c>
       <c r="G38">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H38">
         <v>107</v>
@@ -4160,7 +4160,7 @@
         <v>2273</v>
       </c>
       <c r="G41">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H41">
         <v>105</v>
@@ -4214,7 +4214,7 @@
         <v>2273</v>
       </c>
       <c r="G42">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H42">
         <v>105</v>
@@ -4315,7 +4315,7 @@
         <v>2273</v>
       </c>
       <c r="G43">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H43">
         <v>105</v>
@@ -4369,7 +4369,7 @@
         <v>579</v>
       </c>
       <c r="G44">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H44">
         <v>106</v>
@@ -4473,7 +4473,7 @@
         <v>579</v>
       </c>
       <c r="G45">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H45">
         <v>106</v>

</xml_diff>

<commit_message>
Deployed 681f2eb with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA 12S metab/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
+++ b/eDNA 12S metab/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
@@ -2518,7 +2518,7 @@
         <v>122</v>
       </c>
       <c r="G24">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H24">
         <v>105</v>
@@ -2572,7 +2572,7 @@
         <v>122</v>
       </c>
       <c r="G25">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H25">
         <v>105</v>
@@ -2673,7 +2673,7 @@
         <v>122</v>
       </c>
       <c r="G26">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H26">
         <v>105</v>
@@ -2727,7 +2727,7 @@
         <v>170</v>
       </c>
       <c r="G27">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="H27">
         <v>107</v>
@@ -2831,7 +2831,7 @@
         <v>170</v>
       </c>
       <c r="G28">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="H28">
         <v>107</v>
@@ -2935,7 +2935,7 @@
         <v>170</v>
       </c>
       <c r="G29">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="H29">
         <v>107</v>
@@ -3435,7 +3435,7 @@
         <v>178</v>
       </c>
       <c r="G34">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H34">
         <v>107</v>
@@ -3539,7 +3539,7 @@
         <v>178</v>
       </c>
       <c r="G35">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H35">
         <v>107</v>
@@ -3643,7 +3643,7 @@
         <v>178</v>
       </c>
       <c r="G36">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H36">
         <v>107</v>
@@ -3747,7 +3747,7 @@
         <v>178</v>
       </c>
       <c r="G37">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H37">
         <v>107</v>
@@ -3851,7 +3851,7 @@
         <v>178</v>
       </c>
       <c r="G38">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H38">
         <v>107</v>
@@ -4160,7 +4160,7 @@
         <v>2273</v>
       </c>
       <c r="G41">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H41">
         <v>105</v>
@@ -4214,7 +4214,7 @@
         <v>2273</v>
       </c>
       <c r="G42">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H42">
         <v>105</v>
@@ -4315,7 +4315,7 @@
         <v>2273</v>
       </c>
       <c r="G43">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H43">
         <v>105</v>

</xml_diff>